<commit_message>
update internship details works
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -399,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -723,7 +723,7 @@
         <v>india</v>
       </c>
       <c r="N6" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="O6" t="str">
         <v>Yes</v>

</xml_diff>

<commit_message>
added unknown document upload
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -443,7 +443,7 @@
         <v>Location</v>
       </c>
       <c r="N1" t="str">
-        <v>Offer Letter Submitted</v>
+        <v>Offer Letter</v>
       </c>
       <c r="O1" t="str">
         <v>Completion Certificate</v>
@@ -723,7 +723,7 @@
         <v>india</v>
       </c>
       <c r="N6" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="O6" t="str">
         <v>Yes</v>

</xml_diff>

<commit_message>
fixed google drive api
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -838,9 +838,65 @@
         <v/>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>1234567890123</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Bob</v>
+      </c>
+      <c r="C9" t="str">
+        <v>1234509876</v>
+      </c>
+      <c r="D9" t="str">
+        <v>A</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F9" t="str">
+        <v>3 months</v>
+      </c>
+      <c r="G9" t="str">
+        <v>2025-01-11</v>
+      </c>
+      <c r="H9" t="str">
+        <v>2025-04-23</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Boom Company</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Campus</v>
+      </c>
+      <c r="K9" t="str">
+        <v>123000</v>
+      </c>
+      <c r="L9" t="str">
+        <v>Industry</v>
+      </c>
+      <c r="M9" t="str">
+        <v>Chennai</v>
+      </c>
+      <c r="N9" t="str">
+        <v>No</v>
+      </c>
+      <c r="O9" t="str">
+        <v/>
+      </c>
+      <c r="P9" t="str">
+        <v/>
+      </c>
+      <c r="Q9" t="str">
+        <v/>
+      </c>
+      <c r="R9" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:R8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:R9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>